<commit_message>
Should be working python program, adjusted excel values also implemented in program
</commit_message>
<xml_diff>
--- a/codec_quality_variable_mapping.xlsx
+++ b/codec_quality_variable_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omer Baddour\PycharmProjects\ResearchV3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AA4B15-E53F-44A5-891B-F415460BCF28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4773C223-395B-4CD2-BF2A-9AAD2FDE9237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7257D58B-DD03-4FA5-8F71-E3A1D27441B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Quality</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>up to 20% will notice, otherwise just heard as bad</t>
+  </si>
+  <si>
+    <t>units ms</t>
+  </si>
+  <si>
+    <t>crowd of people talking/screaming/being eaten by monster</t>
+  </si>
+  <si>
+    <t>texas chainsaw masacre movie, emulate sound?</t>
   </si>
 </sst>
 </file>
@@ -135,11 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -456,17 +469,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F195D4-BB0E-44F1-9F8B-AFBDB068346F}">
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="37.81640625" customWidth="1"/>
     <col min="3" max="3" width="46.90625" customWidth="1"/>
-    <col min="4" max="4" width="45.08984375" customWidth="1"/>
+    <col min="4" max="4" width="50.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="31.6328125" bestFit="1" customWidth="1"/>
@@ -510,10 +523,10 @@
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="6"/>
       <c r="D4" t="s">
         <v>11</v>
       </c>
@@ -523,7 +536,7 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>0</v>
       </c>
       <c r="H4">
@@ -541,13 +554,13 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -561,13 +574,13 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>5</v>
       </c>
       <c r="H6" s="4">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -581,13 +594,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="5">
+        <v>10</v>
       </c>
       <c r="H7" s="4">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -601,13 +614,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G8" s="5">
+        <v>10</v>
       </c>
       <c r="H8" s="4">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -621,13 +634,13 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="G9" s="5">
+        <v>15</v>
       </c>
       <c r="H9" s="4">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -641,13 +654,13 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>30</v>
-      </c>
-      <c r="G10">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="G10" s="5">
+        <v>15</v>
       </c>
       <c r="H10" s="4">
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -661,13 +674,13 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>40</v>
-      </c>
-      <c r="G11">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="G11" s="5">
+        <v>20</v>
       </c>
       <c r="H11" s="4">
-        <v>70</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -681,13 +694,13 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>40</v>
-      </c>
-      <c r="G12">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="G12" s="5">
+        <v>20</v>
       </c>
       <c r="H12" s="4">
-        <v>80</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -701,13 +714,13 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>50</v>
-      </c>
-      <c r="G13">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="G13" s="5">
+        <v>25</v>
       </c>
       <c r="H13" s="4">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -721,18 +734,34 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="G14" s="5">
+        <v>25</v>
       </c>
       <c r="H14" s="4">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>